<commit_message>
#9 leiner Read-Test mit 2 Terminen: ein Konzert (Atempause) ohne Ensemble und eine Probe mit 4 singenden Ensembles. Extra Tabellenblatt!
</commit_message>
<xml_diff>
--- a/calendartools/src/test/resources/Gesamtprobenplan_und_ensembles.xlsx
+++ b/calendartools/src/test/resources/Gesamtprobenplan_und_ensembles.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="11748" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CD_2017-12-22" sheetId="2" r:id="rId1"/>
     <sheet name="Ensembles" sheetId="3" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CD_2017-12-22'!$A$1:$W$683</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4696" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4734" uniqueCount="287">
   <si>
     <t>Mo.</t>
   </si>
@@ -1490,7 +1491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1500,9 +1501,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW683"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43231,4 +43232,880 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IW3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:257" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17"/>
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
+      <c r="CB1" s="17"/>
+      <c r="CC1" s="17"/>
+      <c r="CD1" s="17"/>
+      <c r="CE1" s="17"/>
+      <c r="CF1" s="17"/>
+      <c r="CG1" s="17"/>
+      <c r="CH1" s="17"/>
+      <c r="CI1" s="17"/>
+      <c r="CJ1" s="17"/>
+      <c r="CK1" s="17"/>
+      <c r="CL1" s="17"/>
+      <c r="CM1" s="17"/>
+      <c r="CN1" s="17"/>
+      <c r="CO1" s="17"/>
+      <c r="CP1" s="17"/>
+      <c r="CQ1" s="17"/>
+      <c r="CR1" s="17"/>
+      <c r="CS1" s="17"/>
+      <c r="CT1" s="17"/>
+      <c r="CU1" s="17"/>
+      <c r="CV1" s="17"/>
+      <c r="CW1" s="17"/>
+      <c r="CX1" s="17"/>
+      <c r="CY1" s="17"/>
+      <c r="CZ1" s="17"/>
+      <c r="DA1" s="17"/>
+      <c r="DB1" s="17"/>
+      <c r="DC1" s="17"/>
+      <c r="DD1" s="17"/>
+      <c r="DE1" s="17"/>
+      <c r="DF1" s="17"/>
+      <c r="DG1" s="17"/>
+      <c r="DH1" s="17"/>
+      <c r="DI1" s="17"/>
+      <c r="DJ1" s="17"/>
+      <c r="DK1" s="17"/>
+      <c r="DL1" s="17"/>
+      <c r="DM1" s="17"/>
+      <c r="DN1" s="17"/>
+      <c r="DO1" s="17"/>
+      <c r="DP1" s="17"/>
+      <c r="DQ1" s="17"/>
+      <c r="DR1" s="17"/>
+      <c r="DS1" s="17"/>
+      <c r="DT1" s="17"/>
+      <c r="DU1" s="17"/>
+      <c r="DV1" s="17"/>
+      <c r="DW1" s="17"/>
+      <c r="DX1" s="17"/>
+      <c r="DY1" s="17"/>
+      <c r="DZ1" s="17"/>
+      <c r="EA1" s="17"/>
+      <c r="EB1" s="17"/>
+      <c r="EC1" s="17"/>
+      <c r="ED1" s="17"/>
+      <c r="EE1" s="17"/>
+      <c r="EF1" s="17"/>
+      <c r="EG1" s="17"/>
+      <c r="EH1" s="17"/>
+      <c r="EI1" s="17"/>
+      <c r="EJ1" s="17"/>
+      <c r="EK1" s="17"/>
+      <c r="EL1" s="17"/>
+      <c r="EM1" s="17"/>
+      <c r="EN1" s="17"/>
+      <c r="EO1" s="17"/>
+      <c r="EP1" s="17"/>
+      <c r="EQ1" s="17"/>
+      <c r="ER1" s="17"/>
+      <c r="ES1" s="17"/>
+      <c r="ET1" s="17"/>
+      <c r="EU1" s="17"/>
+      <c r="EV1" s="17"/>
+      <c r="EW1" s="17"/>
+      <c r="EX1" s="17"/>
+      <c r="EY1" s="17"/>
+      <c r="EZ1" s="17"/>
+      <c r="FA1" s="17"/>
+      <c r="FB1" s="17"/>
+      <c r="FC1" s="17"/>
+      <c r="FD1" s="17"/>
+      <c r="FE1" s="17"/>
+      <c r="FF1" s="17"/>
+      <c r="FG1" s="17"/>
+      <c r="FH1" s="17"/>
+      <c r="FI1" s="17"/>
+      <c r="FJ1" s="17"/>
+      <c r="FK1" s="17"/>
+      <c r="FL1" s="17"/>
+      <c r="FM1" s="17"/>
+      <c r="FN1" s="17"/>
+      <c r="FO1" s="17"/>
+      <c r="FP1" s="17"/>
+      <c r="FQ1" s="17"/>
+      <c r="FR1" s="17"/>
+      <c r="FS1" s="17"/>
+      <c r="FT1" s="17"/>
+      <c r="FU1" s="17"/>
+      <c r="FV1" s="17"/>
+      <c r="FW1" s="17"/>
+      <c r="FX1" s="17"/>
+      <c r="FY1" s="17"/>
+      <c r="FZ1" s="18"/>
+      <c r="GA1" s="18"/>
+      <c r="GB1" s="18"/>
+      <c r="GC1" s="18"/>
+      <c r="GD1" s="18"/>
+      <c r="GE1" s="18"/>
+      <c r="GF1" s="18"/>
+      <c r="GG1" s="18"/>
+      <c r="GH1" s="18"/>
+      <c r="GI1" s="18"/>
+      <c r="GJ1" s="18"/>
+      <c r="GK1" s="18"/>
+      <c r="GL1" s="18"/>
+      <c r="GM1" s="18"/>
+      <c r="GN1" s="18"/>
+      <c r="GO1" s="18"/>
+      <c r="GP1" s="18"/>
+      <c r="GQ1" s="18"/>
+      <c r="GR1" s="18"/>
+      <c r="GS1" s="18"/>
+      <c r="GT1" s="18"/>
+      <c r="GU1" s="18"/>
+      <c r="GV1" s="18"/>
+      <c r="GW1" s="18"/>
+      <c r="GX1" s="18"/>
+      <c r="GY1" s="18"/>
+      <c r="GZ1" s="18"/>
+      <c r="HA1" s="18"/>
+      <c r="HB1" s="18"/>
+      <c r="HC1" s="18"/>
+      <c r="HD1" s="18"/>
+      <c r="HE1" s="18"/>
+      <c r="HF1" s="18"/>
+      <c r="HG1" s="18"/>
+      <c r="HH1" s="18"/>
+      <c r="HI1" s="18"/>
+      <c r="HJ1" s="18"/>
+      <c r="HK1" s="18"/>
+      <c r="HL1" s="18"/>
+      <c r="HM1" s="18"/>
+      <c r="HN1" s="18"/>
+      <c r="HO1" s="18"/>
+      <c r="HP1" s="18"/>
+      <c r="HQ1" s="18"/>
+      <c r="HR1" s="18"/>
+      <c r="HS1" s="18"/>
+      <c r="HT1" s="18"/>
+      <c r="HU1" s="18"/>
+      <c r="HV1" s="18"/>
+      <c r="HW1" s="18"/>
+      <c r="HX1" s="18"/>
+      <c r="HY1" s="18"/>
+      <c r="HZ1" s="18"/>
+      <c r="IA1" s="18"/>
+      <c r="IB1" s="18"/>
+      <c r="IC1" s="18"/>
+      <c r="ID1" s="18"/>
+      <c r="IE1" s="18"/>
+      <c r="IF1" s="18"/>
+      <c r="IG1" s="18"/>
+      <c r="IH1" s="18"/>
+      <c r="II1" s="18"/>
+      <c r="IJ1" s="18"/>
+      <c r="IK1" s="18"/>
+      <c r="IL1" s="18"/>
+      <c r="IM1" s="18"/>
+      <c r="IN1" s="18"/>
+      <c r="IO1" s="18"/>
+      <c r="IP1" s="18"/>
+      <c r="IQ1" s="18"/>
+      <c r="IR1" s="18"/>
+      <c r="IS1" s="18"/>
+      <c r="IT1" s="18"/>
+      <c r="IU1" s="18"/>
+      <c r="IV1" s="18"/>
+      <c r="IW1" s="18"/>
+    </row>
+    <row r="2" spans="1:257" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43091</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43091</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="10"/>
+      <c r="BL2" s="10"/>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="10"/>
+      <c r="BO2" s="10"/>
+      <c r="BP2" s="10"/>
+      <c r="BQ2" s="10"/>
+      <c r="BR2" s="10"/>
+      <c r="BS2" s="10"/>
+      <c r="BT2" s="10"/>
+      <c r="BU2" s="10"/>
+      <c r="BV2" s="10"/>
+      <c r="BW2" s="10"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10"/>
+      <c r="CC2" s="10"/>
+      <c r="CD2" s="10"/>
+      <c r="CE2" s="10"/>
+      <c r="CF2" s="10"/>
+      <c r="CG2" s="10"/>
+      <c r="CH2" s="10"/>
+      <c r="CI2" s="10"/>
+      <c r="CJ2" s="10"/>
+      <c r="CK2" s="10"/>
+      <c r="CL2" s="10"/>
+      <c r="CM2" s="10"/>
+      <c r="CN2" s="10"/>
+      <c r="CO2" s="10"/>
+      <c r="CP2" s="10"/>
+      <c r="CQ2" s="10"/>
+      <c r="CR2" s="10"/>
+      <c r="CS2" s="10"/>
+      <c r="CT2" s="10"/>
+      <c r="CU2" s="10"/>
+      <c r="CV2" s="10"/>
+      <c r="CW2" s="10"/>
+      <c r="CX2" s="10"/>
+      <c r="CY2" s="10"/>
+      <c r="CZ2" s="10"/>
+      <c r="DA2" s="10"/>
+      <c r="DB2" s="10"/>
+      <c r="DC2" s="10"/>
+      <c r="DD2" s="10"/>
+      <c r="DE2" s="10"/>
+      <c r="DF2" s="10"/>
+      <c r="DG2" s="10"/>
+      <c r="DH2" s="10"/>
+      <c r="DI2" s="10"/>
+      <c r="DJ2" s="10"/>
+      <c r="DK2" s="10"/>
+      <c r="DL2" s="10"/>
+      <c r="DM2" s="10"/>
+      <c r="DN2" s="10"/>
+      <c r="DO2" s="10"/>
+      <c r="DP2" s="10"/>
+      <c r="DQ2" s="10"/>
+      <c r="DR2" s="10"/>
+      <c r="DS2" s="10"/>
+      <c r="DT2" s="10"/>
+      <c r="DU2" s="10"/>
+      <c r="DV2" s="10"/>
+      <c r="DW2" s="10"/>
+      <c r="DX2" s="10"/>
+      <c r="DY2" s="10"/>
+      <c r="DZ2" s="10"/>
+      <c r="EA2" s="10"/>
+      <c r="EB2" s="10"/>
+      <c r="EC2" s="10"/>
+      <c r="ED2" s="10"/>
+      <c r="EE2" s="10"/>
+      <c r="EF2" s="10"/>
+      <c r="EG2" s="10"/>
+      <c r="EH2" s="10"/>
+      <c r="EI2" s="10"/>
+      <c r="EJ2" s="10"/>
+      <c r="EK2" s="10"/>
+      <c r="EL2" s="10"/>
+      <c r="EM2" s="10"/>
+      <c r="EN2" s="10"/>
+      <c r="EO2" s="10"/>
+      <c r="EP2" s="10"/>
+      <c r="EQ2" s="10"/>
+      <c r="ER2" s="10"/>
+      <c r="ES2" s="10"/>
+      <c r="ET2" s="10"/>
+      <c r="EU2" s="10"/>
+      <c r="EV2" s="10"/>
+      <c r="EW2" s="10"/>
+      <c r="EX2" s="10"/>
+      <c r="EY2" s="10"/>
+      <c r="EZ2" s="10"/>
+      <c r="FA2" s="10"/>
+      <c r="FB2" s="10"/>
+      <c r="FC2" s="10"/>
+      <c r="FD2" s="10"/>
+      <c r="FE2" s="10"/>
+      <c r="FF2" s="10"/>
+      <c r="FG2" s="10"/>
+      <c r="FH2" s="10"/>
+      <c r="FI2" s="10"/>
+      <c r="FJ2" s="10"/>
+      <c r="FK2" s="10"/>
+      <c r="FL2" s="10"/>
+      <c r="FM2" s="10"/>
+      <c r="FN2" s="10"/>
+      <c r="FO2" s="10"/>
+      <c r="FP2" s="10"/>
+      <c r="FQ2" s="10"/>
+      <c r="FR2" s="10"/>
+      <c r="FS2" s="10"/>
+      <c r="FT2" s="10"/>
+      <c r="FU2" s="10"/>
+      <c r="FV2" s="10"/>
+      <c r="FW2" s="10"/>
+      <c r="FX2" s="10"/>
+      <c r="FY2" s="10"/>
+      <c r="FZ2" s="20"/>
+      <c r="GA2" s="20"/>
+      <c r="GB2" s="20"/>
+      <c r="GC2" s="20"/>
+      <c r="GD2" s="20"/>
+      <c r="GE2" s="20"/>
+      <c r="GF2" s="20"/>
+      <c r="GG2" s="20"/>
+      <c r="GH2" s="20"/>
+      <c r="GI2" s="20"/>
+      <c r="GJ2" s="20"/>
+      <c r="GK2" s="20"/>
+      <c r="GL2" s="20"/>
+      <c r="GM2" s="20"/>
+      <c r="GN2" s="20"/>
+      <c r="GO2" s="20"/>
+      <c r="GP2" s="20"/>
+      <c r="GQ2" s="20"/>
+      <c r="GR2" s="20"/>
+      <c r="GS2" s="20"/>
+      <c r="GT2" s="20"/>
+      <c r="GU2" s="20"/>
+      <c r="GV2" s="20"/>
+      <c r="GW2" s="20"/>
+      <c r="GX2" s="20"/>
+      <c r="GY2" s="20"/>
+      <c r="GZ2" s="20"/>
+      <c r="HA2" s="20"/>
+      <c r="HB2" s="20"/>
+      <c r="HC2" s="20"/>
+      <c r="HD2" s="20"/>
+      <c r="HE2" s="20"/>
+      <c r="HF2" s="20"/>
+      <c r="HG2" s="20"/>
+      <c r="HH2" s="20"/>
+      <c r="HI2" s="20"/>
+      <c r="HJ2" s="20"/>
+      <c r="HK2" s="20"/>
+      <c r="HL2" s="20"/>
+      <c r="HM2" s="20"/>
+      <c r="HN2" s="20"/>
+      <c r="HO2" s="20"/>
+      <c r="HP2" s="20"/>
+      <c r="HQ2" s="20"/>
+      <c r="HR2" s="20"/>
+      <c r="HS2" s="20"/>
+      <c r="HT2" s="20"/>
+      <c r="HU2" s="20"/>
+      <c r="HV2" s="20"/>
+      <c r="HW2" s="20"/>
+      <c r="HX2" s="20"/>
+      <c r="HY2" s="20"/>
+      <c r="HZ2" s="20"/>
+      <c r="IA2" s="20"/>
+      <c r="IB2" s="20"/>
+      <c r="IC2" s="20"/>
+      <c r="ID2" s="20"/>
+      <c r="IE2" s="20"/>
+      <c r="IF2" s="20"/>
+      <c r="IG2" s="20"/>
+      <c r="IH2" s="20"/>
+      <c r="II2" s="20"/>
+      <c r="IJ2" s="20"/>
+      <c r="IK2" s="20"/>
+      <c r="IL2" s="20"/>
+      <c r="IM2" s="20"/>
+      <c r="IN2" s="20"/>
+      <c r="IO2" s="20"/>
+      <c r="IP2" s="20"/>
+      <c r="IQ2" s="20"/>
+      <c r="IR2" s="20"/>
+      <c r="IS2" s="20"/>
+      <c r="IT2" s="20"/>
+      <c r="IU2" s="20"/>
+      <c r="IV2" s="20"/>
+      <c r="IW2" s="20"/>
+    </row>
+    <row r="3" spans="1:257" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43092</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43092</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10"/>
+      <c r="BA3" s="10"/>
+      <c r="BB3" s="10"/>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10"/>
+      <c r="BE3" s="10"/>
+      <c r="BF3" s="10"/>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10"/>
+      <c r="BI3" s="10"/>
+      <c r="BJ3" s="10"/>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="10"/>
+      <c r="BM3" s="10"/>
+      <c r="BN3" s="10"/>
+      <c r="BO3" s="10"/>
+      <c r="BP3" s="10"/>
+      <c r="BQ3" s="10"/>
+      <c r="BR3" s="10"/>
+      <c r="BS3" s="10"/>
+      <c r="BT3" s="10"/>
+      <c r="BU3" s="10"/>
+      <c r="BV3" s="10"/>
+      <c r="BW3" s="10"/>
+      <c r="BX3" s="10"/>
+      <c r="BY3" s="10"/>
+      <c r="BZ3" s="10"/>
+      <c r="CA3" s="10"/>
+      <c r="CB3" s="10"/>
+      <c r="CC3" s="10"/>
+      <c r="CD3" s="10"/>
+      <c r="CE3" s="10"/>
+      <c r="CF3" s="10"/>
+      <c r="CG3" s="10"/>
+      <c r="CH3" s="10"/>
+      <c r="CI3" s="10"/>
+      <c r="CJ3" s="10"/>
+      <c r="CK3" s="10"/>
+      <c r="CL3" s="10"/>
+      <c r="CM3" s="10"/>
+      <c r="CN3" s="10"/>
+      <c r="CO3" s="10"/>
+      <c r="CP3" s="10"/>
+      <c r="CQ3" s="10"/>
+      <c r="CR3" s="10"/>
+      <c r="CS3" s="10"/>
+      <c r="CT3" s="10"/>
+      <c r="CU3" s="10"/>
+      <c r="CV3" s="10"/>
+      <c r="CW3" s="10"/>
+      <c r="CX3" s="10"/>
+      <c r="CY3" s="10"/>
+      <c r="CZ3" s="10"/>
+      <c r="DA3" s="10"/>
+      <c r="DB3" s="10"/>
+      <c r="DC3" s="10"/>
+      <c r="DD3" s="10"/>
+      <c r="DE3" s="10"/>
+      <c r="DF3" s="10"/>
+      <c r="DG3" s="10"/>
+      <c r="DH3" s="10"/>
+      <c r="DI3" s="10"/>
+      <c r="DJ3" s="10"/>
+      <c r="DK3" s="10"/>
+      <c r="DL3" s="10"/>
+      <c r="DM3" s="10"/>
+      <c r="DN3" s="10"/>
+      <c r="DO3" s="10"/>
+      <c r="DP3" s="10"/>
+      <c r="DQ3" s="10"/>
+      <c r="DR3" s="10"/>
+      <c r="DS3" s="10"/>
+      <c r="DT3" s="10"/>
+      <c r="DU3" s="10"/>
+      <c r="DV3" s="10"/>
+      <c r="DW3" s="10"/>
+      <c r="DX3" s="10"/>
+      <c r="DY3" s="10"/>
+      <c r="DZ3" s="10"/>
+      <c r="EA3" s="10"/>
+      <c r="EB3" s="10"/>
+      <c r="EC3" s="10"/>
+      <c r="ED3" s="10"/>
+      <c r="EE3" s="10"/>
+      <c r="EF3" s="10"/>
+      <c r="EG3" s="10"/>
+      <c r="EH3" s="10"/>
+      <c r="EI3" s="10"/>
+      <c r="EJ3" s="10"/>
+      <c r="EK3" s="10"/>
+      <c r="EL3" s="10"/>
+      <c r="EM3" s="10"/>
+      <c r="EN3" s="10"/>
+      <c r="EO3" s="10"/>
+      <c r="EP3" s="10"/>
+      <c r="EQ3" s="10"/>
+      <c r="ER3" s="10"/>
+      <c r="ES3" s="10"/>
+      <c r="ET3" s="10"/>
+      <c r="EU3" s="10"/>
+      <c r="EV3" s="10"/>
+      <c r="EW3" s="10"/>
+      <c r="EX3" s="10"/>
+      <c r="EY3" s="10"/>
+      <c r="EZ3" s="10"/>
+      <c r="FA3" s="10"/>
+      <c r="FB3" s="10"/>
+      <c r="FC3" s="10"/>
+      <c r="FD3" s="10"/>
+      <c r="FE3" s="10"/>
+      <c r="FF3" s="10"/>
+      <c r="FG3" s="10"/>
+      <c r="FH3" s="10"/>
+      <c r="FI3" s="10"/>
+      <c r="FJ3" s="10"/>
+      <c r="FK3" s="10"/>
+      <c r="FL3" s="10"/>
+      <c r="FM3" s="10"/>
+      <c r="FN3" s="10"/>
+      <c r="FO3" s="10"/>
+      <c r="FP3" s="10"/>
+      <c r="FQ3" s="10"/>
+      <c r="FR3" s="10"/>
+      <c r="FS3" s="10"/>
+      <c r="FT3" s="10"/>
+      <c r="FU3" s="10"/>
+      <c r="FV3" s="10"/>
+      <c r="FW3" s="10"/>
+      <c r="FX3" s="10"/>
+      <c r="FY3" s="10"/>
+      <c r="FZ3" s="20"/>
+      <c r="GA3" s="20"/>
+      <c r="GB3" s="20"/>
+      <c r="GC3" s="20"/>
+      <c r="GD3" s="20"/>
+      <c r="GE3" s="20"/>
+      <c r="GF3" s="20"/>
+      <c r="GG3" s="20"/>
+      <c r="GH3" s="20"/>
+      <c r="GI3" s="20"/>
+      <c r="GJ3" s="20"/>
+      <c r="GK3" s="20"/>
+      <c r="GL3" s="20"/>
+      <c r="GM3" s="20"/>
+      <c r="GN3" s="20"/>
+      <c r="GO3" s="20"/>
+      <c r="GP3" s="20"/>
+      <c r="GQ3" s="20"/>
+      <c r="GR3" s="20"/>
+      <c r="GS3" s="20"/>
+      <c r="GT3" s="20"/>
+      <c r="GU3" s="20"/>
+      <c r="GV3" s="20"/>
+      <c r="GW3" s="20"/>
+      <c r="GX3" s="20"/>
+      <c r="GY3" s="20"/>
+      <c r="GZ3" s="20"/>
+      <c r="HA3" s="20"/>
+      <c r="HB3" s="20"/>
+      <c r="HC3" s="20"/>
+      <c r="HD3" s="20"/>
+      <c r="HE3" s="20"/>
+      <c r="HF3" s="20"/>
+      <c r="HG3" s="20"/>
+      <c r="HH3" s="20"/>
+      <c r="HI3" s="20"/>
+      <c r="HJ3" s="20"/>
+      <c r="HK3" s="20"/>
+      <c r="HL3" s="20"/>
+      <c r="HM3" s="20"/>
+      <c r="HN3" s="20"/>
+      <c r="HO3" s="20"/>
+      <c r="HP3" s="20"/>
+      <c r="HQ3" s="20"/>
+      <c r="HR3" s="20"/>
+      <c r="HS3" s="20"/>
+      <c r="HT3" s="20"/>
+      <c r="HU3" s="20"/>
+      <c r="HV3" s="20"/>
+      <c r="HW3" s="20"/>
+      <c r="HX3" s="20"/>
+      <c r="HY3" s="20"/>
+      <c r="HZ3" s="20"/>
+      <c r="IA3" s="20"/>
+      <c r="IB3" s="20"/>
+      <c r="IC3" s="20"/>
+      <c r="ID3" s="20"/>
+      <c r="IE3" s="20"/>
+      <c r="IF3" s="20"/>
+      <c r="IG3" s="20"/>
+      <c r="IH3" s="20"/>
+      <c r="II3" s="20"/>
+      <c r="IJ3" s="20"/>
+      <c r="IK3" s="20"/>
+      <c r="IL3" s="20"/>
+      <c r="IM3" s="20"/>
+      <c r="IN3" s="20"/>
+      <c r="IO3" s="20"/>
+      <c r="IP3" s="20"/>
+      <c r="IQ3" s="20"/>
+      <c r="IR3" s="20"/>
+      <c r="IS3" s="20"/>
+      <c r="IT3" s="20"/>
+      <c r="IU3" s="20"/>
+      <c r="IV3" s="20"/>
+      <c r="IW3" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>